<commit_message>
util-res-data-prep now works with new and bigger dataset 💖
</commit_message>
<xml_diff>
--- a/util-res-task/monthly_target_date_df_1.xlsx
+++ b/util-res-task/monthly_target_date_df_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E356"/>
+  <dimension ref="A1:E357"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1442-01-01</t>
+          <t>1443-01-01</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -482,7 +482,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1442-01-02</t>
+          <t>1443-01-02</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -501,7 +501,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1442-01-03</t>
+          <t>1443-01-03</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -520,7 +520,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1442-01-04</t>
+          <t>1443-01-04</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -539,7 +539,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1442-01-05</t>
+          <t>1443-01-05</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -558,7 +558,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1442-01-06</t>
+          <t>1443-01-06</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -577,7 +577,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1442-01-07</t>
+          <t>1443-01-07</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -596,7 +596,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1442-01-08</t>
+          <t>1443-01-08</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -615,7 +615,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1442-01-09</t>
+          <t>1443-01-09</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -634,7 +634,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1442-01-10</t>
+          <t>1443-01-10</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -653,7 +653,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1442-01-11</t>
+          <t>1443-01-11</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -672,7 +672,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1442-01-12</t>
+          <t>1443-01-12</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -691,7 +691,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1442-01-13</t>
+          <t>1443-01-13</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -710,7 +710,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1442-01-14</t>
+          <t>1443-01-14</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -729,7 +729,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1442-01-15</t>
+          <t>1443-01-15</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -748,7 +748,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1442-01-16</t>
+          <t>1443-01-16</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -767,7 +767,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1442-01-17</t>
+          <t>1443-01-17</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -786,7 +786,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1442-01-18</t>
+          <t>1443-01-18</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -805,7 +805,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1442-01-19</t>
+          <t>1443-01-19</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -824,7 +824,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1442-01-20</t>
+          <t>1443-01-20</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -843,7 +843,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1442-01-21</t>
+          <t>1443-01-21</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -862,7 +862,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1442-01-22</t>
+          <t>1443-01-22</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -881,7 +881,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1442-01-23</t>
+          <t>1443-01-23</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -900,7 +900,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1442-01-24</t>
+          <t>1443-01-24</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -919,7 +919,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1442-01-25</t>
+          <t>1443-01-25</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -938,7 +938,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1442-01-26</t>
+          <t>1443-01-26</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -957,7 +957,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1442-01-27</t>
+          <t>1443-01-27</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -976,7 +976,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1442-01-28</t>
+          <t>1443-01-28</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -995,7 +995,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1442-01-29</t>
+          <t>1443-01-29</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1014,7 +1014,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1442-02-01</t>
+          <t>1443-01-30</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1033,7 +1033,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1442-02-02</t>
+          <t>1443-02-01</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1052,7 +1052,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1442-02-03</t>
+          <t>1443-02-02</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1071,7 +1071,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1442-02-04</t>
+          <t>1443-02-03</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1090,7 +1090,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1442-02-05</t>
+          <t>1443-02-04</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1109,7 +1109,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1442-02-06</t>
+          <t>1443-02-05</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1128,7 +1128,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1442-02-07</t>
+          <t>1443-02-06</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1147,7 +1147,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1442-02-08</t>
+          <t>1443-02-07</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1166,7 +1166,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1442-02-09</t>
+          <t>1443-02-08</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1185,7 +1185,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1442-02-10</t>
+          <t>1443-02-09</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1204,7 +1204,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>1442-02-11</t>
+          <t>1443-02-10</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1223,7 +1223,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1442-02-12</t>
+          <t>1443-02-11</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1242,7 +1242,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1442-02-13</t>
+          <t>1443-02-12</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1261,7 +1261,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>1442-02-14</t>
+          <t>1443-02-13</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1280,7 +1280,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1442-02-15</t>
+          <t>1443-02-14</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1299,7 +1299,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1442-02-16</t>
+          <t>1443-02-15</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1318,7 +1318,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1442-02-17</t>
+          <t>1443-02-16</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1337,7 +1337,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1442-02-18</t>
+          <t>1443-02-17</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1356,7 +1356,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1442-02-19</t>
+          <t>1443-02-18</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1375,7 +1375,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1442-02-20</t>
+          <t>1443-02-19</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1394,7 +1394,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1442-02-21</t>
+          <t>1443-02-20</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1413,7 +1413,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1442-02-22</t>
+          <t>1443-02-21</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1432,7 +1432,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1442-02-23</t>
+          <t>1443-02-22</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1451,7 +1451,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1442-02-24</t>
+          <t>1443-02-23</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1470,7 +1470,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1442-02-25</t>
+          <t>1443-02-24</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1489,7 +1489,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1442-02-26</t>
+          <t>1443-02-25</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1508,7 +1508,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1442-02-27</t>
+          <t>1443-02-26</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1527,7 +1527,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1442-02-28</t>
+          <t>1443-02-27</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1546,7 +1546,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1442-02-29</t>
+          <t>1443-02-28</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1565,7 +1565,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1442-02-30</t>
+          <t>1443-02-29</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1584,7 +1584,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1442-03-01</t>
+          <t>1443-03-01</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1603,7 +1603,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1442-03-02</t>
+          <t>1443-03-02</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1622,7 +1622,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1442-03-03</t>
+          <t>1443-03-03</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1641,7 +1641,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1442-03-04</t>
+          <t>1443-03-04</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1660,7 +1660,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1442-03-05</t>
+          <t>1443-03-05</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1679,7 +1679,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>1442-03-06</t>
+          <t>1443-03-06</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1698,7 +1698,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>1442-03-07</t>
+          <t>1443-03-07</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1717,7 +1717,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>1442-03-08</t>
+          <t>1443-03-08</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1736,7 +1736,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>1442-03-09</t>
+          <t>1443-03-09</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1755,7 +1755,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>1442-03-10</t>
+          <t>1443-03-10</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1774,7 +1774,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>1442-03-11</t>
+          <t>1443-03-11</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1793,7 +1793,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>1442-03-12</t>
+          <t>1443-03-12</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1812,7 +1812,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>1442-03-13</t>
+          <t>1443-03-13</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1831,7 +1831,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>1442-03-14</t>
+          <t>1443-03-14</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1850,7 +1850,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>1442-03-15</t>
+          <t>1443-03-15</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1869,7 +1869,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>1442-03-16</t>
+          <t>1443-03-16</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1888,7 +1888,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>1442-03-17</t>
+          <t>1443-03-17</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1907,7 +1907,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>1442-03-18</t>
+          <t>1443-03-18</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1926,7 +1926,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>1442-03-19</t>
+          <t>1443-03-19</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1945,7 +1945,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>1442-03-20</t>
+          <t>1443-03-20</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1964,7 +1964,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>1442-03-21</t>
+          <t>1443-03-21</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1983,7 +1983,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>1442-03-22</t>
+          <t>1443-03-22</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -2002,7 +2002,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>1442-03-23</t>
+          <t>1443-03-23</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -2021,7 +2021,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>1442-03-24</t>
+          <t>1443-03-24</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -2040,7 +2040,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>1442-03-25</t>
+          <t>1443-03-25</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -2059,7 +2059,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>1442-03-26</t>
+          <t>1443-03-26</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -2078,7 +2078,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>1442-03-27</t>
+          <t>1443-03-27</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -2097,7 +2097,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>1442-03-28</t>
+          <t>1443-03-28</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -2116,7 +2116,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>1442-03-29</t>
+          <t>1443-03-29</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -2135,7 +2135,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>1442-04-01</t>
+          <t>1443-03-30</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -2154,7 +2154,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>1442-04-02</t>
+          <t>1443-04-01</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -2173,7 +2173,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>1442-04-03</t>
+          <t>1443-04-02</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -2192,7 +2192,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>1442-04-04</t>
+          <t>1443-04-03</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -2211,7 +2211,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>1442-04-05</t>
+          <t>1443-04-04</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -2230,7 +2230,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>1442-04-06</t>
+          <t>1443-04-05</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -2249,7 +2249,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>1442-04-07</t>
+          <t>1443-04-06</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -2268,7 +2268,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>1442-04-08</t>
+          <t>1443-04-07</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -2287,7 +2287,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>1442-04-09</t>
+          <t>1443-04-08</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -2306,7 +2306,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>1442-04-10</t>
+          <t>1443-04-09</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -2325,7 +2325,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>1442-04-11</t>
+          <t>1443-04-10</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -2344,7 +2344,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>1442-04-12</t>
+          <t>1443-04-11</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -2363,7 +2363,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>1442-04-13</t>
+          <t>1443-04-12</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -2382,7 +2382,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>1442-04-14</t>
+          <t>1443-04-13</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -2401,7 +2401,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>1442-04-15</t>
+          <t>1443-04-14</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -2420,7 +2420,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>1442-04-16</t>
+          <t>1443-04-15</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -2439,7 +2439,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>1442-04-17</t>
+          <t>1443-04-16</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -2458,7 +2458,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>1442-04-18</t>
+          <t>1443-04-17</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -2477,7 +2477,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>1442-04-19</t>
+          <t>1443-04-18</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -2496,7 +2496,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>1442-04-20</t>
+          <t>1443-04-19</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -2515,7 +2515,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>1442-04-21</t>
+          <t>1443-04-20</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -2534,7 +2534,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>1442-04-22</t>
+          <t>1443-04-21</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -2553,7 +2553,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>1442-04-23</t>
+          <t>1443-04-22</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -2572,7 +2572,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>1442-04-24</t>
+          <t>1443-04-23</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -2591,7 +2591,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>1442-04-25</t>
+          <t>1443-04-24</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -2610,7 +2610,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>1442-04-26</t>
+          <t>1443-04-25</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -2629,7 +2629,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>1442-04-27</t>
+          <t>1443-04-26</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -2648,7 +2648,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>1442-04-28</t>
+          <t>1443-04-27</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -2667,7 +2667,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>1442-04-29</t>
+          <t>1443-04-28</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -2686,7 +2686,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>1442-04-30</t>
+          <t>1443-04-29</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -2705,7 +2705,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>1442-05-01</t>
+          <t>1443-05-01</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -2724,7 +2724,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>1442-05-02</t>
+          <t>1443-05-02</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -2743,7 +2743,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>1442-05-03</t>
+          <t>1443-05-03</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -2762,7 +2762,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>1442-05-04</t>
+          <t>1443-05-04</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -2781,7 +2781,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>1442-05-05</t>
+          <t>1443-05-05</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -2800,7 +2800,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>1442-05-06</t>
+          <t>1443-05-06</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -2819,7 +2819,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>1442-05-07</t>
+          <t>1443-05-07</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -2838,7 +2838,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>1442-05-08</t>
+          <t>1443-05-08</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -2857,7 +2857,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>1442-05-09</t>
+          <t>1443-05-09</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -2876,7 +2876,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>1442-05-10</t>
+          <t>1443-05-10</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -2895,7 +2895,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>1442-05-11</t>
+          <t>1443-05-11</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -2914,7 +2914,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>1442-05-12</t>
+          <t>1443-05-12</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -2933,7 +2933,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>1442-05-13</t>
+          <t>1443-05-13</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -2952,7 +2952,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>1442-05-14</t>
+          <t>1443-05-14</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -2971,7 +2971,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>1442-05-15</t>
+          <t>1443-05-15</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -2990,11 +2990,11 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>1442-05-16</t>
+          <t>1443-05-16</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C135" t="n">
         <v>0</v>
@@ -3009,7 +3009,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>1442-05-17</t>
+          <t>1443-05-17</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -3028,7 +3028,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>1442-05-18</t>
+          <t>1443-05-18</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -3047,7 +3047,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>1442-05-19</t>
+          <t>1443-05-19</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -3066,7 +3066,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>1442-05-20</t>
+          <t>1443-05-20</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -3085,7 +3085,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>1442-05-21</t>
+          <t>1443-05-21</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -3104,7 +3104,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>1442-05-22</t>
+          <t>1443-05-22</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -3123,7 +3123,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>1442-05-23</t>
+          <t>1443-05-23</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -3142,7 +3142,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>1442-05-24</t>
+          <t>1443-05-24</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -3161,7 +3161,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>1442-05-25</t>
+          <t>1443-05-25</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -3180,7 +3180,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>1442-05-26</t>
+          <t>1443-05-26</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -3199,7 +3199,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>1442-05-27</t>
+          <t>1443-05-27</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -3218,7 +3218,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>1442-05-28</t>
+          <t>1443-05-28</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -3237,7 +3237,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>1442-05-29</t>
+          <t>1443-05-29</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -3256,7 +3256,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>1442-06-01</t>
+          <t>1443-05-30</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -3275,7 +3275,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>1442-06-02</t>
+          <t>1443-06-01</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -3294,7 +3294,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>1442-06-03</t>
+          <t>1443-06-02</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -3313,7 +3313,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>1442-06-04</t>
+          <t>1443-06-03</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -3332,7 +3332,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>1442-06-05</t>
+          <t>1443-06-04</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -3351,7 +3351,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>1442-06-06</t>
+          <t>1443-06-05</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -3370,7 +3370,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>1442-06-07</t>
+          <t>1443-06-06</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -3389,7 +3389,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>1442-06-08</t>
+          <t>1443-06-07</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -3408,7 +3408,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>1442-06-09</t>
+          <t>1443-06-08</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -3427,7 +3427,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>1442-06-10</t>
+          <t>1443-06-09</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -3446,7 +3446,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>1442-06-11</t>
+          <t>1443-06-10</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -3465,7 +3465,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>1442-06-12</t>
+          <t>1443-06-11</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -3484,7 +3484,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>1442-06-13</t>
+          <t>1443-06-12</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -3503,7 +3503,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>1442-06-14</t>
+          <t>1443-06-13</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -3522,7 +3522,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>1442-06-15</t>
+          <t>1443-06-14</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -3541,7 +3541,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>1442-06-16</t>
+          <t>1443-06-15</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -3560,7 +3560,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>1442-06-17</t>
+          <t>1443-06-16</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -3579,7 +3579,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>1442-06-18</t>
+          <t>1443-06-17</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -3598,7 +3598,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>1442-06-19</t>
+          <t>1443-06-18</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -3617,7 +3617,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>1442-06-20</t>
+          <t>1443-06-19</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -3636,7 +3636,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>1442-06-21</t>
+          <t>1443-06-20</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -3655,7 +3655,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>1442-06-22</t>
+          <t>1443-06-21</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -3674,7 +3674,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>1442-06-23</t>
+          <t>1443-06-22</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -3693,7 +3693,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>1442-06-24</t>
+          <t>1443-06-23</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -3712,7 +3712,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>1442-06-25</t>
+          <t>1443-06-24</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -3731,7 +3731,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>1442-06-26</t>
+          <t>1443-06-25</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -3750,7 +3750,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>1442-06-27</t>
+          <t>1443-06-26</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -3769,7 +3769,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>1442-06-28</t>
+          <t>1443-06-27</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -3788,7 +3788,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>1442-06-29</t>
+          <t>1443-06-28</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -3807,11 +3807,11 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>1442-06-30</t>
+          <t>1443-06-29</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C178" t="n">
         <v>0</v>
@@ -3826,7 +3826,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>1442-07-01</t>
+          <t>1443-07-01</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -3845,7 +3845,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>1442-07-02</t>
+          <t>1443-07-02</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -3864,7 +3864,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>1442-07-03</t>
+          <t>1443-07-03</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -3883,7 +3883,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>1442-07-04</t>
+          <t>1443-07-04</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -3902,7 +3902,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>1442-07-05</t>
+          <t>1443-07-05</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -3921,11 +3921,11 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>1442-07-06</t>
+          <t>1443-07-06</t>
         </is>
       </c>
       <c r="B184" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C184" t="n">
         <v>0</v>
@@ -3940,11 +3940,11 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>1442-07-07</t>
+          <t>1443-07-07</t>
         </is>
       </c>
       <c r="B185" t="n">
-        <v>0</v>
+        <v>649</v>
       </c>
       <c r="C185" t="n">
         <v>0</v>
@@ -3959,7 +3959,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>1442-07-08</t>
+          <t>1443-07-08</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -3978,7 +3978,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>1442-07-09</t>
+          <t>1443-07-09</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -3997,7 +3997,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>1442-07-10</t>
+          <t>1443-07-10</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -4016,11 +4016,11 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>1442-07-11</t>
+          <t>1443-07-11</t>
         </is>
       </c>
       <c r="B189" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C189" t="n">
         <v>0</v>
@@ -4035,7 +4035,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>1442-07-12</t>
+          <t>1443-07-12</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -4054,7 +4054,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>1442-07-13</t>
+          <t>1443-07-13</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -4073,11 +4073,11 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>1442-07-14</t>
+          <t>1443-07-14</t>
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C192" t="n">
         <v>0</v>
@@ -4092,7 +4092,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>1442-07-15</t>
+          <t>1443-07-15</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -4111,7 +4111,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>1442-07-16</t>
+          <t>1443-07-16</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -4130,7 +4130,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>1442-07-17</t>
+          <t>1443-07-17</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -4149,11 +4149,11 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>1442-07-18</t>
+          <t>1443-07-18</t>
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C196" t="n">
         <v>0</v>
@@ -4168,11 +4168,11 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>1442-07-19</t>
+          <t>1443-07-19</t>
         </is>
       </c>
       <c r="B197" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C197" t="n">
         <v>0</v>
@@ -4187,11 +4187,11 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>1442-07-20</t>
+          <t>1443-07-20</t>
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="C198" t="n">
         <v>0</v>
@@ -4206,14 +4206,14 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>1442-07-21</t>
+          <t>1443-07-21</t>
         </is>
       </c>
       <c r="B199" t="n">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="C199" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D199" t="n">
         <v>0</v>
@@ -4225,7 +4225,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>1442-07-22</t>
+          <t>1443-07-22</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -4244,7 +4244,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>1442-07-23</t>
+          <t>1443-07-23</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -4263,7 +4263,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>1442-07-24</t>
+          <t>1443-07-24</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -4282,11 +4282,11 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>1442-07-25</t>
+          <t>1443-07-25</t>
         </is>
       </c>
       <c r="B203" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C203" t="n">
         <v>0</v>
@@ -4301,11 +4301,11 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>1442-07-26</t>
+          <t>1443-07-26</t>
         </is>
       </c>
       <c r="B204" t="n">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="C204" t="n">
         <v>0</v>
@@ -4320,7 +4320,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>1442-07-27</t>
+          <t>1443-07-27</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -4339,11 +4339,11 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>1442-07-28</t>
+          <t>1443-07-28</t>
         </is>
       </c>
       <c r="B206" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C206" t="n">
         <v>0</v>
@@ -4358,11 +4358,11 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>1442-07-29</t>
+          <t>1443-07-29</t>
         </is>
       </c>
       <c r="B207" t="n">
-        <v>0</v>
+        <v>453</v>
       </c>
       <c r="C207" t="n">
         <v>0</v>
@@ -4377,11 +4377,11 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>1442-08-01</t>
+          <t>1443-07-30</t>
         </is>
       </c>
       <c r="B208" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C208" t="n">
         <v>0</v>
@@ -4396,11 +4396,11 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>1442-08-02</t>
+          <t>1443-08-01</t>
         </is>
       </c>
       <c r="B209" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C209" t="n">
         <v>0</v>
@@ -4415,11 +4415,11 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>1442-08-03</t>
+          <t>1443-08-02</t>
         </is>
       </c>
       <c r="B210" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C210" t="n">
         <v>0</v>
@@ -4434,11 +4434,11 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>1442-08-04</t>
+          <t>1443-08-03</t>
         </is>
       </c>
       <c r="B211" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C211" t="n">
         <v>0</v>
@@ -4453,11 +4453,11 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>1442-08-05</t>
+          <t>1443-08-04</t>
         </is>
       </c>
       <c r="B212" t="n">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="C212" t="n">
         <v>0</v>
@@ -4472,11 +4472,11 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>1442-08-06</t>
+          <t>1443-08-05</t>
         </is>
       </c>
       <c r="B213" t="n">
-        <v>0</v>
+        <v>292</v>
       </c>
       <c r="C213" t="n">
         <v>0</v>
@@ -4491,14 +4491,14 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>1442-08-07</t>
+          <t>1443-08-06</t>
         </is>
       </c>
       <c r="B214" t="n">
-        <v>0</v>
+        <v>273</v>
       </c>
       <c r="C214" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D214" t="n">
         <v>0</v>
@@ -4510,14 +4510,14 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>1442-08-08</t>
+          <t>1443-08-07</t>
         </is>
       </c>
       <c r="B215" t="n">
-        <v>0</v>
+        <v>1720</v>
       </c>
       <c r="C215" t="n">
-        <v>0</v>
+        <v>445</v>
       </c>
       <c r="D215" t="n">
         <v>0</v>
@@ -4529,11 +4529,11 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>1442-08-09</t>
+          <t>1443-08-08</t>
         </is>
       </c>
       <c r="B216" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="C216" t="n">
         <v>0</v>
@@ -4548,14 +4548,14 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>1442-08-10</t>
+          <t>1443-08-09</t>
         </is>
       </c>
       <c r="B217" t="n">
-        <v>0</v>
+        <v>2013</v>
       </c>
       <c r="C217" t="n">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="D217" t="n">
         <v>0</v>
@@ -4567,14 +4567,14 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>1442-08-11</t>
+          <t>1443-08-10</t>
         </is>
       </c>
       <c r="B218" t="n">
-        <v>0</v>
+        <v>844</v>
       </c>
       <c r="C218" t="n">
-        <v>0</v>
+        <v>321</v>
       </c>
       <c r="D218" t="n">
         <v>0</v>
@@ -4586,14 +4586,14 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>1442-08-12</t>
+          <t>1443-08-11</t>
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0</v>
+        <v>1179</v>
       </c>
       <c r="C219" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D219" t="n">
         <v>0</v>
@@ -4605,14 +4605,14 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>1442-08-13</t>
+          <t>1443-08-12</t>
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0</v>
+        <v>1947</v>
       </c>
       <c r="C220" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D220" t="n">
         <v>0</v>
@@ -4624,14 +4624,14 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>1442-08-14</t>
+          <t>1443-08-13</t>
         </is>
       </c>
       <c r="B221" t="n">
-        <v>12</v>
+        <v>1434</v>
       </c>
       <c r="C221" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D221" t="n">
         <v>0</v>
@@ -4643,14 +4643,14 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>1442-08-15</t>
+          <t>1443-08-14</t>
         </is>
       </c>
       <c r="B222" t="n">
-        <v>0</v>
+        <v>1089</v>
       </c>
       <c r="C222" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="D222" t="n">
         <v>0</v>
@@ -4662,11 +4662,11 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>1442-08-16</t>
+          <t>1443-08-15</t>
         </is>
       </c>
       <c r="B223" t="n">
-        <v>0</v>
+        <v>362</v>
       </c>
       <c r="C223" t="n">
         <v>0</v>
@@ -4681,14 +4681,14 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>1442-08-17</t>
+          <t>1443-08-16</t>
         </is>
       </c>
       <c r="B224" t="n">
-        <v>0</v>
+        <v>3727</v>
       </c>
       <c r="C224" t="n">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D224" t="n">
         <v>0</v>
@@ -4700,14 +4700,14 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>1442-08-18</t>
+          <t>1443-08-17</t>
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0</v>
+        <v>1980</v>
       </c>
       <c r="C225" t="n">
-        <v>0</v>
+        <v>1229</v>
       </c>
       <c r="D225" t="n">
         <v>0</v>
@@ -4719,14 +4719,14 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>1442-08-19</t>
+          <t>1443-08-18</t>
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0</v>
+        <v>1322</v>
       </c>
       <c r="C226" t="n">
-        <v>0</v>
+        <v>2488</v>
       </c>
       <c r="D226" t="n">
         <v>0</v>
@@ -4738,11 +4738,11 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>1442-08-20</t>
+          <t>1443-08-19</t>
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="C227" t="n">
         <v>0</v>
@@ -4757,14 +4757,14 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>1442-08-21</t>
+          <t>1443-08-20</t>
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0</v>
+        <v>916</v>
       </c>
       <c r="C228" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D228" t="n">
         <v>0</v>
@@ -4776,14 +4776,14 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>1442-08-22</t>
+          <t>1443-08-21</t>
         </is>
       </c>
       <c r="B229" t="n">
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="C229" t="n">
-        <v>0</v>
+        <v>1096</v>
       </c>
       <c r="D229" t="n">
         <v>0</v>
@@ -4795,11 +4795,11 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>1442-08-23</t>
+          <t>1443-08-22</t>
         </is>
       </c>
       <c r="B230" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C230" t="n">
         <v>0</v>
@@ -4814,14 +4814,14 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>1442-08-24</t>
+          <t>1443-08-23</t>
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0</v>
+        <v>1278</v>
       </c>
       <c r="C231" t="n">
-        <v>0</v>
+        <v>766</v>
       </c>
       <c r="D231" t="n">
         <v>0</v>
@@ -4833,17 +4833,17 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>1442-08-25</t>
+          <t>1443-08-24</t>
         </is>
       </c>
       <c r="B232" t="n">
-        <v>0</v>
+        <v>1295</v>
       </c>
       <c r="C232" t="n">
-        <v>0</v>
+        <v>9366</v>
       </c>
       <c r="D232" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="E232" t="n">
         <v>0</v>
@@ -4852,14 +4852,14 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>1442-08-26</t>
+          <t>1443-08-25</t>
         </is>
       </c>
       <c r="B233" t="n">
-        <v>0</v>
+        <v>1608</v>
       </c>
       <c r="C233" t="n">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="D233" t="n">
         <v>0</v>
@@ -4871,14 +4871,14 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>1442-08-27</t>
+          <t>1443-08-26</t>
         </is>
       </c>
       <c r="B234" t="n">
-        <v>0</v>
+        <v>1549</v>
       </c>
       <c r="C234" t="n">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="D234" t="n">
         <v>0</v>
@@ -4890,14 +4890,14 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>1442-08-28</t>
+          <t>1443-08-27</t>
         </is>
       </c>
       <c r="B235" t="n">
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="C235" t="n">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="D235" t="n">
         <v>0</v>
@@ -4909,14 +4909,14 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>1442-08-29</t>
+          <t>1443-08-28</t>
         </is>
       </c>
       <c r="B236" t="n">
-        <v>0</v>
+        <v>1166</v>
       </c>
       <c r="C236" t="n">
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="D236" t="n">
         <v>0</v>
@@ -4928,14 +4928,14 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>1442-08-30</t>
+          <t>1443-08-29</t>
         </is>
       </c>
       <c r="B237" t="n">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="C237" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D237" t="n">
         <v>0</v>
@@ -4947,14 +4947,14 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>1442-09-01</t>
+          <t>1443-09-01</t>
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0</v>
+        <v>948</v>
       </c>
       <c r="C238" t="n">
-        <v>0</v>
+        <v>442</v>
       </c>
       <c r="D238" t="n">
         <v>0</v>
@@ -4966,14 +4966,14 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>1442-09-02</t>
+          <t>1443-09-02</t>
         </is>
       </c>
       <c r="B239" t="n">
-        <v>0</v>
+        <v>1111</v>
       </c>
       <c r="C239" t="n">
-        <v>0</v>
+        <v>424</v>
       </c>
       <c r="D239" t="n">
         <v>0</v>
@@ -4985,17 +4985,17 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>1442-09-03</t>
+          <t>1443-09-03</t>
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0</v>
+        <v>738</v>
       </c>
       <c r="C240" t="n">
-        <v>0</v>
+        <v>394</v>
       </c>
       <c r="D240" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="E240" t="n">
         <v>0</v>
@@ -5004,14 +5004,14 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>1442-09-04</t>
+          <t>1443-09-04</t>
         </is>
       </c>
       <c r="B241" t="n">
-        <v>4</v>
+        <v>967</v>
       </c>
       <c r="C241" t="n">
-        <v>0</v>
+        <v>623</v>
       </c>
       <c r="D241" t="n">
         <v>0</v>
@@ -5023,14 +5023,14 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>1442-09-05</t>
+          <t>1443-09-05</t>
         </is>
       </c>
       <c r="B242" t="n">
-        <v>3</v>
+        <v>757</v>
       </c>
       <c r="C242" t="n">
-        <v>0</v>
+        <v>556</v>
       </c>
       <c r="D242" t="n">
         <v>0</v>
@@ -5042,14 +5042,14 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>1442-09-06</t>
+          <t>1443-09-06</t>
         </is>
       </c>
       <c r="B243" t="n">
-        <v>3</v>
+        <v>756</v>
       </c>
       <c r="C243" t="n">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="D243" t="n">
         <v>0</v>
@@ -5061,14 +5061,14 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>1442-09-07</t>
+          <t>1443-09-07</t>
         </is>
       </c>
       <c r="B244" t="n">
-        <v>3</v>
+        <v>299</v>
       </c>
       <c r="C244" t="n">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="D244" t="n">
         <v>0</v>
@@ -5080,14 +5080,14 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>1442-09-08</t>
+          <t>1443-09-08</t>
         </is>
       </c>
       <c r="B245" t="n">
-        <v>3</v>
+        <v>776</v>
       </c>
       <c r="C245" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D245" t="n">
         <v>0</v>
@@ -5099,14 +5099,14 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>1442-09-09</t>
+          <t>1443-09-09</t>
         </is>
       </c>
       <c r="B246" t="n">
-        <v>3</v>
+        <v>406</v>
       </c>
       <c r="C246" t="n">
-        <v>0</v>
+        <v>2409</v>
       </c>
       <c r="D246" t="n">
         <v>0</v>
@@ -5118,14 +5118,14 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>1442-09-10</t>
+          <t>1443-09-10</t>
         </is>
       </c>
       <c r="B247" t="n">
-        <v>3</v>
+        <v>649</v>
       </c>
       <c r="C247" t="n">
-        <v>0</v>
+        <v>877</v>
       </c>
       <c r="D247" t="n">
         <v>0</v>
@@ -5137,14 +5137,14 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>1442-09-11</t>
+          <t>1443-09-11</t>
         </is>
       </c>
       <c r="B248" t="n">
-        <v>3</v>
+        <v>830</v>
       </c>
       <c r="C248" t="n">
-        <v>0</v>
+        <v>321</v>
       </c>
       <c r="D248" t="n">
         <v>0</v>
@@ -5156,12 +5156,14 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>1442-09-12</t>
-        </is>
-      </c>
-      <c r="B249" t="inlineStr"/>
+          <t>1443-09-12</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>697</v>
+      </c>
       <c r="C249" t="n">
-        <v>0</v>
+        <v>435</v>
       </c>
       <c r="D249" t="n">
         <v>0</v>
@@ -5173,15 +5175,17 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>1442-09-13</t>
-        </is>
-      </c>
-      <c r="B250" t="inlineStr"/>
+          <t>1443-09-13</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>952</v>
+      </c>
       <c r="C250" t="n">
-        <v>0</v>
+        <v>1590</v>
       </c>
       <c r="D250" t="n">
-        <v>0</v>
+        <v>959</v>
       </c>
       <c r="E250" t="n">
         <v>0</v>
@@ -5190,12 +5194,14 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>1442-09-14</t>
-        </is>
-      </c>
-      <c r="B251" t="inlineStr"/>
+          <t>1443-09-14</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>319</v>
+      </c>
       <c r="C251" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D251" t="n">
         <v>0</v>
@@ -5207,12 +5213,14 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>1442-09-15</t>
-        </is>
-      </c>
-      <c r="B252" t="inlineStr"/>
+          <t>1443-09-15</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>572</v>
+      </c>
       <c r="C252" t="n">
-        <v>0</v>
+        <v>1852</v>
       </c>
       <c r="D252" t="n">
         <v>0</v>
@@ -5224,15 +5232,17 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>1442-09-16</t>
-        </is>
-      </c>
-      <c r="B253" t="inlineStr"/>
+          <t>1443-09-16</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>512</v>
+      </c>
       <c r="C253" t="n">
-        <v>0</v>
+        <v>896</v>
       </c>
       <c r="D253" t="n">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="E253" t="n">
         <v>0</v>
@@ -5241,12 +5251,14 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>1442-09-17</t>
-        </is>
-      </c>
-      <c r="B254" t="inlineStr"/>
+          <t>1443-09-17</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>492</v>
+      </c>
       <c r="C254" t="n">
-        <v>0</v>
+        <v>2004</v>
       </c>
       <c r="D254" t="n">
         <v>0</v>
@@ -5258,12 +5270,14 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>1442-09-18</t>
-        </is>
-      </c>
-      <c r="B255" t="inlineStr"/>
+          <t>1443-09-18</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>593</v>
+      </c>
       <c r="C255" t="n">
-        <v>0</v>
+        <v>1044</v>
       </c>
       <c r="D255" t="n">
         <v>0</v>
@@ -5275,15 +5289,17 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>1442-09-19</t>
-        </is>
-      </c>
-      <c r="B256" t="inlineStr"/>
+          <t>1443-09-19</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>594</v>
+      </c>
       <c r="C256" t="n">
-        <v>0</v>
+        <v>1840</v>
       </c>
       <c r="D256" t="n">
-        <v>0</v>
+        <v>630</v>
       </c>
       <c r="E256" t="n">
         <v>0</v>
@@ -5292,15 +5308,17 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>1442-09-20</t>
-        </is>
-      </c>
-      <c r="B257" t="inlineStr"/>
+          <t>1443-09-20</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>1202</v>
+      </c>
       <c r="C257" t="n">
-        <v>0</v>
+        <v>783</v>
       </c>
       <c r="D257" t="n">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="E257" t="n">
         <v>0</v>
@@ -5309,12 +5327,14 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>1442-09-21</t>
-        </is>
-      </c>
-      <c r="B258" t="inlineStr"/>
+          <t>1443-09-21</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>834</v>
+      </c>
       <c r="C258" t="n">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="D258" t="n">
         <v>0</v>
@@ -5326,15 +5346,17 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>1442-09-22</t>
-        </is>
-      </c>
-      <c r="B259" t="inlineStr"/>
+          <t>1443-09-22</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>703</v>
+      </c>
       <c r="C259" t="n">
-        <v>0</v>
+        <v>488</v>
       </c>
       <c r="D259" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E259" t="n">
         <v>0</v>
@@ -5343,15 +5365,17 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>1442-09-23</t>
-        </is>
-      </c>
-      <c r="B260" t="inlineStr"/>
+          <t>1443-09-23</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>155</v>
+      </c>
       <c r="C260" t="n">
-        <v>0</v>
+        <v>1574</v>
       </c>
       <c r="D260" t="n">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="E260" t="n">
         <v>0</v>
@@ -5360,12 +5384,14 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>1442-09-24</t>
-        </is>
-      </c>
-      <c r="B261" t="inlineStr"/>
+          <t>1443-09-24</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>237</v>
+      </c>
       <c r="C261" t="n">
-        <v>0</v>
+        <v>1030</v>
       </c>
       <c r="D261" t="n">
         <v>0</v>
@@ -5377,15 +5403,17 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>1442-09-25</t>
-        </is>
-      </c>
-      <c r="B262" t="inlineStr"/>
+          <t>1443-09-25</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>19</v>
+      </c>
       <c r="C262" t="n">
-        <v>0</v>
+        <v>1865</v>
       </c>
       <c r="D262" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E262" t="n">
         <v>0</v>
@@ -5394,12 +5422,14 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>1442-09-26</t>
-        </is>
-      </c>
-      <c r="B263" t="inlineStr"/>
+          <t>1443-09-26</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>99</v>
+      </c>
       <c r="C263" t="n">
-        <v>0</v>
+        <v>1083</v>
       </c>
       <c r="D263" t="n">
         <v>0</v>
@@ -5411,15 +5441,17 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>1442-09-27</t>
-        </is>
-      </c>
-      <c r="B264" t="inlineStr"/>
+          <t>1443-09-27</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>75</v>
+      </c>
       <c r="C264" t="n">
-        <v>0</v>
+        <v>590</v>
       </c>
       <c r="D264" t="n">
-        <v>0</v>
+        <v>341</v>
       </c>
       <c r="E264" t="n">
         <v>0</v>
@@ -5428,12 +5460,14 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>1442-09-28</t>
-        </is>
-      </c>
-      <c r="B265" t="inlineStr"/>
+          <t>1443-09-28</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>36</v>
+      </c>
       <c r="C265" t="n">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="D265" t="n">
         <v>0</v>
@@ -5445,15 +5479,17 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>1442-09-29</t>
-        </is>
-      </c>
-      <c r="B266" t="inlineStr"/>
+          <t>1443-09-29</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>85</v>
+      </c>
       <c r="C266" t="n">
-        <v>0</v>
+        <v>963</v>
       </c>
       <c r="D266" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="E266" t="n">
         <v>0</v>
@@ -5462,12 +5498,14 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>1442-09-30</t>
-        </is>
-      </c>
-      <c r="B267" t="inlineStr"/>
+          <t>1443-09-30</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>96</v>
+      </c>
       <c r="C267" t="n">
-        <v>0</v>
+        <v>582</v>
       </c>
       <c r="D267" t="n">
         <v>0</v>
@@ -5479,12 +5517,14 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>1442-10-01</t>
-        </is>
-      </c>
-      <c r="B268" t="inlineStr"/>
+          <t>1443-10-01</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>7</v>
+      </c>
       <c r="C268" t="n">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="D268" t="n">
         <v>0</v>
@@ -5496,12 +5536,14 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>1442-10-02</t>
-        </is>
-      </c>
-      <c r="B269" t="inlineStr"/>
+          <t>1443-10-02</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>1</v>
+      </c>
       <c r="C269" t="n">
-        <v>0</v>
+        <v>409</v>
       </c>
       <c r="D269" t="n">
         <v>0</v>
@@ -5513,12 +5555,14 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>1442-10-03</t>
-        </is>
-      </c>
-      <c r="B270" t="inlineStr"/>
+          <t>1443-10-03</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>0</v>
+      </c>
       <c r="C270" t="n">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="D270" t="n">
         <v>0</v>
@@ -5530,29 +5574,33 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>1442-10-04</t>
-        </is>
-      </c>
-      <c r="B271" t="inlineStr"/>
+          <t>1443-10-04</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>0</v>
+      </c>
       <c r="C271" t="n">
-        <v>0</v>
+        <v>980</v>
       </c>
       <c r="D271" t="n">
-        <v>0</v>
+        <v>286</v>
       </c>
       <c r="E271" t="n">
-        <v>0</v>
+        <v>310</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>1442-10-05</t>
-        </is>
-      </c>
-      <c r="B272" t="inlineStr"/>
+          <t>1443-10-05</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>0</v>
+      </c>
       <c r="C272" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="D272" t="n">
         <v>0</v>
@@ -5564,15 +5612,17 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>1442-10-06</t>
-        </is>
-      </c>
-      <c r="B273" t="inlineStr"/>
+          <t>1443-10-06</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>0</v>
+      </c>
       <c r="C273" t="n">
-        <v>0</v>
+        <v>784</v>
       </c>
       <c r="D273" t="n">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="E273" t="n">
         <v>0</v>
@@ -5581,49 +5631,55 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>1442-10-07</t>
-        </is>
-      </c>
-      <c r="B274" t="inlineStr"/>
+          <t>1443-10-07</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>3</v>
+      </c>
       <c r="C274" t="n">
-        <v>0</v>
+        <v>445</v>
       </c>
       <c r="D274" t="n">
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="E274" t="n">
-        <v>0</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>1442-10-08</t>
-        </is>
-      </c>
-      <c r="B275" t="inlineStr"/>
+          <t>1443-10-08</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>3</v>
+      </c>
       <c r="C275" t="n">
-        <v>0</v>
+        <v>760</v>
       </c>
       <c r="D275" t="n">
-        <v>0</v>
+        <v>7058</v>
       </c>
       <c r="E275" t="n">
-        <v>0</v>
+        <v>5368</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>1442-10-09</t>
-        </is>
-      </c>
-      <c r="B276" t="inlineStr"/>
+          <t>1443-10-09</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>9</v>
+      </c>
       <c r="C276" t="n">
-        <v>0</v>
+        <v>1087</v>
       </c>
       <c r="D276" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="E276" t="n">
         <v>0</v>
@@ -5632,49 +5688,55 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>1442-10-10</t>
-        </is>
-      </c>
-      <c r="B277" t="inlineStr"/>
+          <t>1443-10-10</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>13</v>
+      </c>
       <c r="C277" t="n">
-        <v>0</v>
+        <v>987</v>
       </c>
       <c r="D277" t="n">
-        <v>0</v>
+        <v>214</v>
       </c>
       <c r="E277" t="n">
-        <v>0</v>
+        <v>349</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>1442-10-11</t>
-        </is>
-      </c>
-      <c r="B278" t="inlineStr"/>
+          <t>1443-10-11</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>0</v>
+      </c>
       <c r="C278" t="n">
-        <v>0</v>
+        <v>437</v>
       </c>
       <c r="D278" t="n">
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="E278" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>1442-10-12</t>
-        </is>
-      </c>
-      <c r="B279" t="inlineStr"/>
+          <t>1443-10-12</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>0</v>
+      </c>
       <c r="C279" t="n">
-        <v>0</v>
+        <v>293</v>
       </c>
       <c r="D279" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E279" t="n">
         <v>0</v>
@@ -5683,60 +5745,74 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>1442-10-13</t>
-        </is>
-      </c>
-      <c r="B280" t="inlineStr"/>
+          <t>1443-10-13</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>0</v>
+      </c>
       <c r="C280" t="n">
-        <v>8</v>
+        <v>481</v>
       </c>
       <c r="D280" t="n">
-        <v>0</v>
+        <v>10089</v>
       </c>
       <c r="E280" t="n">
-        <v>0</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>1442-10-14</t>
-        </is>
-      </c>
-      <c r="B281" t="inlineStr"/>
-      <c r="C281" t="inlineStr"/>
+          <t>1443-10-14</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>0</v>
+      </c>
+      <c r="C281" t="n">
+        <v>396</v>
+      </c>
       <c r="D281" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E281" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>1442-10-15</t>
-        </is>
-      </c>
-      <c r="B282" t="inlineStr"/>
-      <c r="C282" t="inlineStr"/>
+          <t>1443-10-15</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>9</v>
+      </c>
+      <c r="C282" t="n">
+        <v>252</v>
+      </c>
       <c r="D282" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E282" t="n">
-        <v>0</v>
+        <v>528</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>1442-10-16</t>
-        </is>
-      </c>
-      <c r="B283" t="inlineStr"/>
-      <c r="C283" t="inlineStr"/>
+          <t>1443-10-16</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>40</v>
+      </c>
+      <c r="C283" t="n">
+        <v>375</v>
+      </c>
       <c r="D283" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E283" t="n">
         <v>0</v>
@@ -5745,43 +5821,55 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>1442-10-17</t>
-        </is>
-      </c>
-      <c r="B284" t="inlineStr"/>
-      <c r="C284" t="inlineStr"/>
+          <t>1443-10-17</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>0</v>
+      </c>
+      <c r="C284" t="n">
+        <v>302</v>
+      </c>
       <c r="D284" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E284" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>1442-10-18</t>
-        </is>
-      </c>
-      <c r="B285" t="inlineStr"/>
-      <c r="C285" t="inlineStr"/>
+          <t>1443-10-18</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>3</v>
+      </c>
+      <c r="C285" t="n">
+        <v>345</v>
+      </c>
       <c r="D285" t="n">
-        <v>0</v>
+        <v>319</v>
       </c>
       <c r="E285" t="n">
-        <v>0</v>
+        <v>717</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>1442-10-19</t>
-        </is>
-      </c>
-      <c r="B286" t="inlineStr"/>
-      <c r="C286" t="inlineStr"/>
+          <t>1443-10-19</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>0</v>
+      </c>
+      <c r="C286" t="n">
+        <v>249</v>
+      </c>
       <c r="D286" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E286" t="n">
         <v>0</v>
@@ -5790,13 +5878,17 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>1442-10-20</t>
-        </is>
-      </c>
-      <c r="B287" t="inlineStr"/>
-      <c r="C287" t="inlineStr"/>
+          <t>1443-10-20</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>0</v>
+      </c>
+      <c r="C287" t="n">
+        <v>261</v>
+      </c>
       <c r="D287" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="E287" t="n">
         <v>0</v>
@@ -5805,13 +5897,17 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>1442-10-21</t>
-        </is>
-      </c>
-      <c r="B288" t="inlineStr"/>
-      <c r="C288" t="inlineStr"/>
+          <t>1443-10-21</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>10</v>
+      </c>
+      <c r="C288" t="n">
+        <v>524</v>
+      </c>
       <c r="D288" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="E288" t="n">
         <v>0</v>
@@ -5820,73 +5916,93 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>1442-10-22</t>
-        </is>
-      </c>
-      <c r="B289" t="inlineStr"/>
-      <c r="C289" t="inlineStr"/>
+          <t>1443-10-22</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>0</v>
+      </c>
+      <c r="C289" t="n">
+        <v>347</v>
+      </c>
       <c r="D289" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="E289" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>1442-10-23</t>
-        </is>
-      </c>
-      <c r="B290" t="inlineStr"/>
-      <c r="C290" t="inlineStr"/>
+          <t>1443-10-23</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>0</v>
+      </c>
+      <c r="C290" t="n">
+        <v>271</v>
+      </c>
       <c r="D290" t="n">
-        <v>0</v>
+        <v>1127</v>
       </c>
       <c r="E290" t="n">
-        <v>0</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>1442-10-24</t>
-        </is>
-      </c>
-      <c r="B291" t="inlineStr"/>
-      <c r="C291" t="inlineStr"/>
+          <t>1443-10-24</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>0</v>
+      </c>
+      <c r="C291" t="n">
+        <v>124</v>
+      </c>
       <c r="D291" t="n">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="E291" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>1442-10-25</t>
-        </is>
-      </c>
-      <c r="B292" t="inlineStr"/>
-      <c r="C292" t="inlineStr"/>
+          <t>1443-10-25</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>0</v>
+      </c>
+      <c r="C292" t="n">
+        <v>84</v>
+      </c>
       <c r="D292" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="E292" t="n">
-        <v>0</v>
+        <v>153</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>1442-10-26</t>
-        </is>
-      </c>
-      <c r="B293" t="inlineStr"/>
-      <c r="C293" t="inlineStr"/>
+          <t>1443-10-26</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>0</v>
+      </c>
+      <c r="C293" t="n">
+        <v>64</v>
+      </c>
       <c r="D293" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E293" t="n">
         <v>0</v>
@@ -5895,103 +6011,131 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>1442-10-27</t>
-        </is>
-      </c>
-      <c r="B294" t="inlineStr"/>
-      <c r="C294" t="inlineStr"/>
+          <t>1443-10-27</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>0</v>
+      </c>
+      <c r="C294" t="n">
+        <v>67</v>
+      </c>
       <c r="D294" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="E294" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>1442-10-28</t>
-        </is>
-      </c>
-      <c r="B295" t="inlineStr"/>
-      <c r="C295" t="inlineStr"/>
+          <t>1443-10-28</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>0</v>
+      </c>
+      <c r="C295" t="n">
+        <v>13</v>
+      </c>
       <c r="D295" t="n">
-        <v>0</v>
+        <v>605</v>
       </c>
       <c r="E295" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>1442-10-29</t>
-        </is>
-      </c>
-      <c r="B296" t="inlineStr"/>
-      <c r="C296" t="inlineStr"/>
+          <t>1443-10-29</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>1290</v>
+      </c>
+      <c r="C296" t="n">
+        <v>28</v>
+      </c>
       <c r="D296" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E296" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>1442-11-01</t>
-        </is>
-      </c>
-      <c r="B297" t="inlineStr"/>
-      <c r="C297" t="inlineStr"/>
+          <t>1443-11-01</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>0</v>
+      </c>
+      <c r="C297" t="n">
+        <v>3</v>
+      </c>
       <c r="D297" t="n">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="E297" t="n">
-        <v>0</v>
+        <v>151</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>1442-11-02</t>
-        </is>
-      </c>
-      <c r="B298" t="inlineStr"/>
-      <c r="C298" t="inlineStr"/>
+          <t>1443-11-02</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>0</v>
+      </c>
+      <c r="C298" t="n">
+        <v>0</v>
+      </c>
       <c r="D298" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="E298" t="n">
-        <v>0</v>
+        <v>174</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>1442-11-03</t>
-        </is>
-      </c>
-      <c r="B299" t="inlineStr"/>
-      <c r="C299" t="inlineStr"/>
+          <t>1443-11-03</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>0</v>
+      </c>
+      <c r="C299" t="n">
+        <v>0</v>
+      </c>
       <c r="D299" t="n">
-        <v>0</v>
+        <v>314</v>
       </c>
       <c r="E299" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>1442-11-04</t>
-        </is>
-      </c>
-      <c r="B300" t="inlineStr"/>
-      <c r="C300" t="inlineStr"/>
+          <t>1443-11-04</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>0</v>
+      </c>
+      <c r="C300" t="n">
+        <v>0</v>
+      </c>
       <c r="D300" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E300" t="n">
         <v>0</v>
@@ -6000,103 +6144,117 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>1442-11-05</t>
-        </is>
-      </c>
-      <c r="B301" t="inlineStr"/>
-      <c r="C301" t="inlineStr"/>
+          <t>1443-11-05</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>0</v>
+      </c>
+      <c r="C301" t="n">
+        <v>0</v>
+      </c>
       <c r="D301" t="n">
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="E301" t="n">
-        <v>0</v>
+        <v>316</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>1442-11-06</t>
-        </is>
-      </c>
-      <c r="B302" t="inlineStr"/>
-      <c r="C302" t="inlineStr"/>
+          <t>1443-11-06</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>22</v>
+      </c>
+      <c r="C302" t="n">
+        <v>42</v>
+      </c>
       <c r="D302" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E302" t="n">
-        <v>0</v>
+        <v>167</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>1442-11-07</t>
-        </is>
-      </c>
-      <c r="B303" t="inlineStr"/>
+          <t>1443-11-07</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>355</v>
+      </c>
       <c r="C303" t="inlineStr"/>
       <c r="D303" t="n">
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="E303" t="n">
-        <v>0</v>
+        <v>154</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>1442-11-08</t>
-        </is>
-      </c>
-      <c r="B304" t="inlineStr"/>
+          <t>1443-11-08</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>2</v>
+      </c>
       <c r="C304" t="inlineStr"/>
       <c r="D304" t="n">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="E304" t="n">
-        <v>0</v>
+        <v>575</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>1442-11-09</t>
-        </is>
-      </c>
-      <c r="B305" t="inlineStr"/>
+          <t>1443-11-09</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>10</v>
+      </c>
       <c r="C305" t="inlineStr"/>
       <c r="D305" t="n">
-        <v>0</v>
+        <v>226</v>
       </c>
       <c r="E305" t="n">
-        <v>0</v>
+        <v>295</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>1442-11-10</t>
+          <t>1443-11-10</t>
         </is>
       </c>
       <c r="B306" t="inlineStr"/>
       <c r="C306" t="inlineStr"/>
       <c r="D306" t="n">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="E306" t="n">
-        <v>0</v>
+        <v>660</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>1442-11-11</t>
+          <t>1443-11-11</t>
         </is>
       </c>
       <c r="B307" t="inlineStr"/>
       <c r="C307" t="inlineStr"/>
       <c r="D307" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="E307" t="n">
         <v>0</v>
@@ -6105,262 +6263,262 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>1442-11-12</t>
+          <t>1443-11-12</t>
         </is>
       </c>
       <c r="B308" t="inlineStr"/>
       <c r="C308" t="inlineStr"/>
       <c r="D308" t="n">
-        <v>0</v>
+        <v>742</v>
       </c>
       <c r="E308" t="n">
-        <v>0</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>1442-11-13</t>
+          <t>1443-11-13</t>
         </is>
       </c>
       <c r="B309" t="inlineStr"/>
       <c r="C309" t="inlineStr"/>
       <c r="D309" t="n">
-        <v>0</v>
+        <v>909</v>
       </c>
       <c r="E309" t="n">
-        <v>0</v>
+        <v>850</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>1442-11-14</t>
+          <t>1443-11-14</t>
         </is>
       </c>
       <c r="B310" t="inlineStr"/>
       <c r="C310" t="inlineStr"/>
       <c r="D310" t="n">
-        <v>0</v>
+        <v>1513</v>
       </c>
       <c r="E310" t="n">
-        <v>0</v>
+        <v>415</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>1442-11-15</t>
+          <t>1443-11-15</t>
         </is>
       </c>
       <c r="B311" t="inlineStr"/>
       <c r="C311" t="inlineStr"/>
       <c r="D311" t="n">
-        <v>0</v>
+        <v>2091</v>
       </c>
       <c r="E311" t="n">
-        <v>0</v>
+        <v>634</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>1442-11-16</t>
+          <t>1443-11-16</t>
         </is>
       </c>
       <c r="B312" t="inlineStr"/>
       <c r="C312" t="inlineStr"/>
       <c r="D312" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E312" t="n">
-        <v>0</v>
+        <v>256</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>1442-11-17</t>
+          <t>1443-11-17</t>
         </is>
       </c>
       <c r="B313" t="inlineStr"/>
       <c r="C313" t="inlineStr"/>
       <c r="D313" t="n">
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="E313" t="n">
-        <v>0</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>1442-11-18</t>
+          <t>1443-11-18</t>
         </is>
       </c>
       <c r="B314" t="inlineStr"/>
       <c r="C314" t="inlineStr"/>
       <c r="D314" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E314" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>1442-11-19</t>
+          <t>1443-11-19</t>
         </is>
       </c>
       <c r="B315" t="inlineStr"/>
       <c r="C315" t="inlineStr"/>
       <c r="D315" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E315" t="n">
-        <v>0</v>
+        <v>780</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>1442-11-20</t>
+          <t>1443-11-20</t>
         </is>
       </c>
       <c r="B316" t="inlineStr"/>
       <c r="C316" t="inlineStr"/>
       <c r="D316" t="n">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="E316" t="n">
-        <v>0</v>
+        <v>334</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>1442-11-21</t>
+          <t>1443-11-21</t>
         </is>
       </c>
       <c r="B317" t="inlineStr"/>
       <c r="C317" t="inlineStr"/>
       <c r="D317" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="E317" t="n">
-        <v>0</v>
+        <v>586</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>1442-11-22</t>
+          <t>1443-11-22</t>
         </is>
       </c>
       <c r="B318" t="inlineStr"/>
       <c r="C318" t="inlineStr"/>
       <c r="D318" t="n">
-        <v>0</v>
+        <v>509</v>
       </c>
       <c r="E318" t="n">
-        <v>0</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>1442-11-23</t>
+          <t>1443-11-23</t>
         </is>
       </c>
       <c r="B319" t="inlineStr"/>
       <c r="C319" t="inlineStr"/>
       <c r="D319" t="n">
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="E319" t="n">
-        <v>0</v>
+        <v>229</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>1442-11-24</t>
+          <t>1443-11-24</t>
         </is>
       </c>
       <c r="B320" t="inlineStr"/>
       <c r="C320" t="inlineStr"/>
       <c r="D320" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="E320" t="n">
-        <v>0</v>
+        <v>292</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>1442-11-25</t>
+          <t>1443-11-25</t>
         </is>
       </c>
       <c r="B321" t="inlineStr"/>
       <c r="C321" t="inlineStr"/>
       <c r="D321" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E321" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>1442-11-26</t>
+          <t>1443-11-26</t>
         </is>
       </c>
       <c r="B322" t="inlineStr"/>
       <c r="C322" t="inlineStr"/>
       <c r="D322" t="n">
-        <v>0</v>
+        <v>268</v>
       </c>
       <c r="E322" t="n">
-        <v>0</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>1442-11-27</t>
+          <t>1443-11-27</t>
         </is>
       </c>
       <c r="B323" t="inlineStr"/>
       <c r="C323" t="inlineStr"/>
       <c r="D323" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E323" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>1442-11-28</t>
+          <t>1443-11-28</t>
         </is>
       </c>
       <c r="B324" t="inlineStr"/>
       <c r="C324" t="inlineStr"/>
       <c r="D324" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="E324" t="n">
-        <v>0</v>
+        <v>341</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>1442-11-29</t>
+          <t>1443-11-29</t>
         </is>
       </c>
       <c r="B325" t="inlineStr"/>
@@ -6369,473 +6527,426 @@
         <v>0</v>
       </c>
       <c r="E325" t="n">
-        <v>0</v>
+        <v>257</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>1442-11-30</t>
+          <t>1443-11-30</t>
         </is>
       </c>
       <c r="B326" t="inlineStr"/>
       <c r="C326" t="inlineStr"/>
       <c r="D326" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E326" t="n">
-        <v>0</v>
+        <v>477</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>1442-12-01</t>
+          <t>1443-12-01</t>
         </is>
       </c>
       <c r="B327" t="inlineStr"/>
       <c r="C327" t="inlineStr"/>
       <c r="D327" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E327" t="n">
-        <v>0</v>
+        <v>284</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>1442-12-02</t>
+          <t>1443-12-02</t>
         </is>
       </c>
       <c r="B328" t="inlineStr"/>
       <c r="C328" t="inlineStr"/>
-      <c r="D328" t="n">
-        <v>0</v>
-      </c>
+      <c r="D328" t="inlineStr"/>
       <c r="E328" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>1442-12-03</t>
+          <t>1443-12-03</t>
         </is>
       </c>
       <c r="B329" t="inlineStr"/>
       <c r="C329" t="inlineStr"/>
-      <c r="D329" t="n">
-        <v>0</v>
-      </c>
+      <c r="D329" t="inlineStr"/>
       <c r="E329" t="n">
-        <v>0</v>
+        <v>436</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>1442-12-04</t>
+          <t>1443-12-04</t>
         </is>
       </c>
       <c r="B330" t="inlineStr"/>
       <c r="C330" t="inlineStr"/>
-      <c r="D330" t="n">
-        <v>0</v>
-      </c>
+      <c r="D330" t="inlineStr"/>
       <c r="E330" t="n">
-        <v>0</v>
+        <v>308</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>1442-12-05</t>
+          <t>1443-12-05</t>
         </is>
       </c>
       <c r="B331" t="inlineStr"/>
       <c r="C331" t="inlineStr"/>
-      <c r="D331" t="n">
-        <v>0</v>
-      </c>
+      <c r="D331" t="inlineStr"/>
       <c r="E331" t="n">
-        <v>0</v>
+        <v>655</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>1442-12-06</t>
+          <t>1443-12-06</t>
         </is>
       </c>
       <c r="B332" t="inlineStr"/>
       <c r="C332" t="inlineStr"/>
-      <c r="D332" t="n">
-        <v>0</v>
-      </c>
+      <c r="D332" t="inlineStr"/>
       <c r="E332" t="n">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>1442-12-07</t>
+          <t>1443-12-07</t>
         </is>
       </c>
       <c r="B333" t="inlineStr"/>
       <c r="C333" t="inlineStr"/>
-      <c r="D333" t="n">
-        <v>0</v>
-      </c>
+      <c r="D333" t="inlineStr"/>
       <c r="E333" t="n">
-        <v>0</v>
+        <v>601</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>1442-12-08</t>
+          <t>1443-12-08</t>
         </is>
       </c>
       <c r="B334" t="inlineStr"/>
       <c r="C334" t="inlineStr"/>
-      <c r="D334" t="n">
-        <v>0</v>
-      </c>
+      <c r="D334" t="inlineStr"/>
       <c r="E334" t="n">
-        <v>0</v>
+        <v>427</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>1442-12-09</t>
+          <t>1443-12-09</t>
         </is>
       </c>
       <c r="B335" t="inlineStr"/>
       <c r="C335" t="inlineStr"/>
-      <c r="D335" t="n">
-        <v>0</v>
-      </c>
+      <c r="D335" t="inlineStr"/>
       <c r="E335" t="n">
-        <v>0</v>
+        <v>323</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>1442-12-10</t>
+          <t>1443-12-10</t>
         </is>
       </c>
       <c r="B336" t="inlineStr"/>
       <c r="C336" t="inlineStr"/>
-      <c r="D336" t="n">
-        <v>0</v>
-      </c>
+      <c r="D336" t="inlineStr"/>
       <c r="E336" t="n">
-        <v>0</v>
+        <v>193</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>1442-12-11</t>
+          <t>1443-12-11</t>
         </is>
       </c>
       <c r="B337" t="inlineStr"/>
       <c r="C337" t="inlineStr"/>
-      <c r="D337" t="n">
-        <v>0</v>
-      </c>
+      <c r="D337" t="inlineStr"/>
       <c r="E337" t="n">
-        <v>0</v>
+        <v>324</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>1442-12-12</t>
+          <t>1443-12-12</t>
         </is>
       </c>
       <c r="B338" t="inlineStr"/>
       <c r="C338" t="inlineStr"/>
-      <c r="D338" t="n">
-        <v>0</v>
-      </c>
+      <c r="D338" t="inlineStr"/>
       <c r="E338" t="n">
-        <v>0</v>
+        <v>416</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>1442-12-13</t>
+          <t>1443-12-13</t>
         </is>
       </c>
       <c r="B339" t="inlineStr"/>
       <c r="C339" t="inlineStr"/>
-      <c r="D339" t="n">
-        <v>0</v>
-      </c>
+      <c r="D339" t="inlineStr"/>
       <c r="E339" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>1442-12-14</t>
+          <t>1443-12-14</t>
         </is>
       </c>
       <c r="B340" t="inlineStr"/>
       <c r="C340" t="inlineStr"/>
-      <c r="D340" t="n">
-        <v>0</v>
-      </c>
+      <c r="D340" t="inlineStr"/>
       <c r="E340" t="n">
-        <v>0</v>
+        <v>408</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>1442-12-15</t>
+          <t>1443-12-15</t>
         </is>
       </c>
       <c r="B341" t="inlineStr"/>
       <c r="C341" t="inlineStr"/>
-      <c r="D341" t="n">
-        <v>0</v>
-      </c>
+      <c r="D341" t="inlineStr"/>
       <c r="E341" t="n">
-        <v>0</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>1442-12-16</t>
+          <t>1443-12-16</t>
         </is>
       </c>
       <c r="B342" t="inlineStr"/>
       <c r="C342" t="inlineStr"/>
-      <c r="D342" t="n">
-        <v>0</v>
-      </c>
+      <c r="D342" t="inlineStr"/>
       <c r="E342" t="n">
-        <v>0</v>
+        <v>318</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>1442-12-17</t>
+          <t>1443-12-17</t>
         </is>
       </c>
       <c r="B343" t="inlineStr"/>
       <c r="C343" t="inlineStr"/>
-      <c r="D343" t="n">
-        <v>0</v>
-      </c>
+      <c r="D343" t="inlineStr"/>
       <c r="E343" t="n">
-        <v>0</v>
+        <v>511</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>1442-12-18</t>
+          <t>1443-12-18</t>
         </is>
       </c>
       <c r="B344" t="inlineStr"/>
       <c r="C344" t="inlineStr"/>
-      <c r="D344" t="n">
-        <v>0</v>
-      </c>
+      <c r="D344" t="inlineStr"/>
       <c r="E344" t="n">
-        <v>0</v>
+        <v>430</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>1442-12-19</t>
+          <t>1443-12-19</t>
         </is>
       </c>
       <c r="B345" t="inlineStr"/>
       <c r="C345" t="inlineStr"/>
-      <c r="D345" t="n">
-        <v>0</v>
-      </c>
+      <c r="D345" t="inlineStr"/>
       <c r="E345" t="n">
-        <v>0</v>
+        <v>354</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>1442-12-20</t>
+          <t>1443-12-20</t>
         </is>
       </c>
       <c r="B346" t="inlineStr"/>
       <c r="C346" t="inlineStr"/>
-      <c r="D346" t="n">
-        <v>0</v>
-      </c>
+      <c r="D346" t="inlineStr"/>
       <c r="E346" t="n">
-        <v>0</v>
+        <v>420</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>1442-12-21</t>
+          <t>1443-12-21</t>
         </is>
       </c>
       <c r="B347" t="inlineStr"/>
       <c r="C347" t="inlineStr"/>
-      <c r="D347" t="n">
-        <v>0</v>
-      </c>
+      <c r="D347" t="inlineStr"/>
       <c r="E347" t="n">
-        <v>0</v>
+        <v>139</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>1442-12-22</t>
+          <t>1443-12-22</t>
         </is>
       </c>
       <c r="B348" t="inlineStr"/>
       <c r="C348" t="inlineStr"/>
-      <c r="D348" t="n">
-        <v>0</v>
-      </c>
+      <c r="D348" t="inlineStr"/>
       <c r="E348" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>1442-12-23</t>
+          <t>1443-12-23</t>
         </is>
       </c>
       <c r="B349" t="inlineStr"/>
       <c r="C349" t="inlineStr"/>
-      <c r="D349" t="n">
-        <v>0</v>
-      </c>
+      <c r="D349" t="inlineStr"/>
       <c r="E349" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>1442-12-24</t>
+          <t>1443-12-24</t>
         </is>
       </c>
       <c r="B350" t="inlineStr"/>
       <c r="C350" t="inlineStr"/>
-      <c r="D350" t="n">
-        <v>0</v>
-      </c>
+      <c r="D350" t="inlineStr"/>
       <c r="E350" t="n">
-        <v>0</v>
+        <v>131</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>1442-12-25</t>
+          <t>1443-12-25</t>
         </is>
       </c>
       <c r="B351" t="inlineStr"/>
       <c r="C351" t="inlineStr"/>
-      <c r="D351" t="n">
-        <v>0</v>
-      </c>
+      <c r="D351" t="inlineStr"/>
       <c r="E351" t="n">
-        <v>0</v>
+        <v>131</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>1442-12-26</t>
+          <t>1443-12-26</t>
         </is>
       </c>
       <c r="B352" t="inlineStr"/>
       <c r="C352" t="inlineStr"/>
-      <c r="D352" t="n">
-        <v>0</v>
-      </c>
+      <c r="D352" t="inlineStr"/>
       <c r="E352" t="n">
-        <v>0</v>
+        <v>131</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>1442-12-27</t>
+          <t>1443-12-27</t>
         </is>
       </c>
       <c r="B353" t="inlineStr"/>
       <c r="C353" t="inlineStr"/>
-      <c r="D353" t="n">
-        <v>0</v>
-      </c>
+      <c r="D353" t="inlineStr"/>
       <c r="E353" t="n">
-        <v>0</v>
+        <v>131</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>1442-12-28</t>
+          <t>1443-12-28</t>
         </is>
       </c>
       <c r="B354" t="inlineStr"/>
       <c r="C354" t="inlineStr"/>
-      <c r="D354" t="n">
-        <v>0</v>
-      </c>
+      <c r="D354" t="inlineStr"/>
       <c r="E354" t="n">
-        <v>0</v>
+        <v>131</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>1442-12-29</t>
+          <t>1443-12-29</t>
         </is>
       </c>
       <c r="B355" t="inlineStr"/>
       <c r="C355" t="inlineStr"/>
-      <c r="D355" t="n">
-        <v>0</v>
-      </c>
+      <c r="D355" t="inlineStr"/>
       <c r="E355" t="n">
-        <v>0</v>
+        <v>131</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>1443-01-01</t>
+          <t>1443-12-30</t>
         </is>
       </c>
       <c r="B356" t="inlineStr"/>
       <c r="C356" t="inlineStr"/>
-      <c r="D356" t="n">
-        <v>0</v>
-      </c>
+      <c r="D356" t="inlineStr"/>
       <c r="E356" t="n">
-        <v>0</v>
-      </c>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1444-01-01</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr"/>
+      <c r="C357" t="inlineStr"/>
+      <c r="D357" t="inlineStr"/>
+      <c r="E357" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>